<commit_message>
git edit.cshtml image previously selected preview corrected
</commit_message>
<xml_diff>
--- a/wwwroot/Uploads/B1B1B020.xlsx
+++ b/wwwroot/Uploads/B1B1B020.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="268">
   <si>
     <r>
       <t>EMPLOYEE CODE</t>
@@ -998,12 +998,6 @@
   </si>
   <si>
     <t>Wife</t>
-  </si>
-  <si>
-    <t>C.ANANDHI</t>
-  </si>
-  <si>
-    <t>Mother</t>
   </si>
   <si>
     <t>M.Sc.</t>
@@ -1819,7 +1813,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1829,8 +1823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GR2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="GA1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="AU2" sqref="AU2:AZ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1873,7 +1867,7 @@
   <sheetData>
     <row r="1" spans="1:200" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1885,10 +1879,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
@@ -1936,16 +1930,16 @@
         <v>17</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="X1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="Z1" s="2" t="s">
         <v>19</v>
@@ -1960,7 +1954,7 @@
         <v>22</v>
       </c>
       <c r="AD1" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="AE1" s="2" t="s">
         <v>23</v>
@@ -1975,7 +1969,7 @@
         <v>26</v>
       </c>
       <c r="AI1" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AJ1" s="2" t="s">
         <v>27</v>
@@ -2020,13 +2014,13 @@
         <v>40</v>
       </c>
       <c r="AX1" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="AY1" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
         <v>257</v>
-      </c>
-      <c r="AY1" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="AZ1" s="2" t="s">
-        <v>259</v>
       </c>
       <c r="BA1" s="2" t="s">
         <v>41</v>
@@ -2287,25 +2281,25 @@
         <v>126</v>
       </c>
       <c r="EI1" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="EJ1" s="2" t="s">
         <v>127</v>
       </c>
       <c r="EK1" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="EL1" s="1" t="s">
         <v>128</v>
       </c>
       <c r="EM1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="EN1" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="EO1" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="EN1" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="EO1" s="1" t="s">
-        <v>264</v>
       </c>
       <c r="EP1" s="1" t="s">
         <v>129</v>
@@ -2323,13 +2317,13 @@
         <v>133</v>
       </c>
       <c r="EU1" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="EV1" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="EW1" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="EV1" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="EW1" s="1" t="s">
-        <v>267</v>
       </c>
       <c r="EX1" s="1" t="s">
         <v>134</v>
@@ -2359,7 +2353,7 @@
         <v>142</v>
       </c>
       <c r="FG1" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="FH1" s="1" t="s">
         <v>143</v>
@@ -2470,12 +2464,12 @@
         <v>178</v>
       </c>
       <c r="GR1" s="12" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:200" s="11" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B2" s="6">
         <v>50003</v>
@@ -2499,7 +2493,7 @@
         <v>184</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>185</v>
@@ -2511,13 +2505,13 @@
         <v>544100534208</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>187</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>188</v>
@@ -2526,7 +2520,7 @@
         <v>48635</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="S2" s="5"/>
       <c r="T2" s="7">
@@ -2608,24 +2602,12 @@
       <c r="AT2" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="AU2" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="AV2" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="AW2" s="5">
-        <v>7448324095</v>
-      </c>
-      <c r="AX2" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="AY2" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="AZ2" s="5">
-        <v>9095671166</v>
-      </c>
+      <c r="AU2" s="4"/>
+      <c r="AV2" s="5"/>
+      <c r="AW2" s="5"/>
+      <c r="AX2" s="4"/>
+      <c r="AY2" s="5"/>
+      <c r="AZ2" s="5"/>
       <c r="BA2" s="4"/>
       <c r="BB2" s="4"/>
       <c r="BC2" s="5"/>
@@ -2645,10 +2627,10 @@
         <v>7448324095</v>
       </c>
       <c r="BM2" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="BN2" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="BO2" s="8">
         <v>0.77500000000000002</v>
@@ -2657,13 +2639,13 @@
         <v>2013</v>
       </c>
       <c r="BQ2" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="BR2" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="BS2" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="BT2" s="8">
         <v>0.66600000000000004</v>
@@ -2672,10 +2654,10 @@
         <v>2008</v>
       </c>
       <c r="BV2" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="BW2" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="BX2" s="8">
         <v>0.77749999999999997</v>
@@ -2684,10 +2666,10 @@
         <v>2004</v>
       </c>
       <c r="BZ2" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="CA2" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="CB2" s="8">
         <v>0.73</v>
@@ -2696,43 +2678,43 @@
         <v>2002</v>
       </c>
       <c r="CD2" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="CE2" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="CF2" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="CG2" s="8">
         <v>0.97</v>
       </c>
       <c r="CH2" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="CI2" s="5">
         <v>2008</v>
       </c>
       <c r="CJ2" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="CK2" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="CL2" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="CM2" s="9">
         <v>0.78</v>
       </c>
       <c r="CN2" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="CO2" s="5">
         <v>2005</v>
       </c>
       <c r="CP2" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="CQ2" s="5"/>
       <c r="CR2" s="5"/>
@@ -2746,7 +2728,7 @@
         <v>13.3</v>
       </c>
       <c r="CX2" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="CY2" s="7">
         <v>41885</v>
@@ -2755,10 +2737,10 @@
         <v>42338</v>
       </c>
       <c r="DA2" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="DB2" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="DC2" s="7">
         <v>41531</v>
@@ -2767,10 +2749,10 @@
         <v>41881</v>
       </c>
       <c r="DE2" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="DF2" s="10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="DG2" s="7">
         <v>39578</v>
@@ -2779,7 +2761,7 @@
         <v>40704</v>
       </c>
       <c r="DI2" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="DJ2" s="5"/>
       <c r="DK2" s="7">
@@ -2829,53 +2811,53 @@
         <v>240000</v>
       </c>
       <c r="EE2" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="EF2" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="EG2" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="EH2" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="EF2" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="EG2" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="EH2" s="5" t="s">
-        <v>219</v>
-      </c>
       <c r="EI2" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="EJ2" s="7">
         <v>41881</v>
       </c>
       <c r="EK2" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="EL2" s="5"/>
       <c r="EM2" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="EN2" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="EN2" s="5" t="s">
-        <v>246</v>
-      </c>
       <c r="EO2" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="EP2" s="6">
         <v>50100343061900</v>
       </c>
       <c r="EQ2" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="ER2" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="ES2" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="ET2" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="EU2" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="EV2" s="5"/>
       <c r="EW2" s="5"/>
@@ -2894,10 +2876,10 @@
         <v>100675663821</v>
       </c>
       <c r="FF2" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="FG2" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="FH2" s="5"/>
       <c r="FI2" s="5">
@@ -2913,22 +2895,22 @@
         <v>0</v>
       </c>
       <c r="FM2" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="FN2" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="FO2" s="5">
         <v>7358714068</v>
       </c>
       <c r="FP2" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="FQ2" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="FR2" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="FS2" s="5"/>
       <c r="FT2" s="5"/>
@@ -2939,25 +2921,25 @@
       <c r="FY2" s="5"/>
       <c r="FZ2" s="5"/>
       <c r="GA2" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="GB2" s="5"/>
       <c r="GC2" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="GD2" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="GE2" s="5"/>
       <c r="GF2" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="GG2" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="GH2" s="5"/>
       <c r="GI2" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="GJ2" s="7">
         <v>41881</v>

</xml_diff>

<commit_message>
marks obtained fields changed null into 0.0
</commit_message>
<xml_diff>
--- a/wwwroot/Uploads/B1B1B020.xlsx
+++ b/wwwroot/Uploads/B1B1B020.xlsx
@@ -1481,7 +1481,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
@@ -1526,6 +1526,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1823,8 +1827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GR2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="AU2" sqref="AU2:AZ2"/>
+    <sheetView tabSelected="1" topLeftCell="CD1" workbookViewId="0">
+      <selection activeCell="CU2" sqref="CU2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2722,7 +2726,7 @@
         <v>0.78</v>
       </c>
       <c r="CT2" s="5"/>
-      <c r="CU2" s="5"/>
+      <c r="CU2" s="14"/>
       <c r="CV2" s="5"/>
       <c r="CW2" s="5">
         <v>13.3</v>

</xml_diff>

<commit_message>
Edit Images Part and Experience round off changes in controller and edit.cshtml
</commit_message>
<xml_diff>
--- a/wwwroot/Uploads/B1B1B020.xlsx
+++ b/wwwroot/Uploads/B1B1B020.xlsx
@@ -1817,7 +1817,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1827,8 +1827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GR2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CD1" workbookViewId="0">
-      <selection activeCell="CU2" sqref="CU2"/>
+    <sheetView tabSelected="1" topLeftCell="DO1" workbookViewId="0">
+      <selection activeCell="DS2" sqref="DS2:EC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2784,33 +2784,17 @@
       </c>
       <c r="DQ2" s="5"/>
       <c r="DR2" s="5"/>
-      <c r="DS2" s="7">
-        <v>31940</v>
-      </c>
-      <c r="DT2" s="7">
-        <v>31940</v>
-      </c>
+      <c r="DS2" s="7"/>
+      <c r="DT2" s="7"/>
       <c r="DU2" s="5"/>
-      <c r="DV2" s="7">
-        <v>31940</v>
-      </c>
-      <c r="DW2" s="7">
-        <v>31940</v>
-      </c>
+      <c r="DV2" s="7"/>
+      <c r="DW2" s="7"/>
       <c r="DX2" s="5"/>
-      <c r="DY2" s="7">
-        <v>31940</v>
-      </c>
-      <c r="DZ2" s="7">
-        <v>31940</v>
-      </c>
+      <c r="DY2" s="7"/>
+      <c r="DZ2" s="7"/>
       <c r="EA2" s="5"/>
-      <c r="EB2" s="7">
-        <v>31940</v>
-      </c>
-      <c r="EC2" s="7">
-        <v>31940</v>
-      </c>
+      <c r="EB2" s="7"/>
+      <c r="EC2" s="7"/>
       <c r="ED2" s="5">
         <v>240000</v>
       </c>

</xml_diff>